<commit_message>
Added date and part of username.
</commit_message>
<xml_diff>
--- a/src/Excel_files/tasks_content.xlsx
+++ b/src/Excel_files/tasks_content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Python\PyCreateTask_Phabricator\Excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Python\PyCreateTask_Phabricator\src\Excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="446">
   <si>
     <t>Module</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1346,114 +1346,6 @@
     <t>我是详情23</t>
   </si>
   <si>
-    <t>E1_plus</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>E2_plus</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>E3_plus</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>E4_plus</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>E5_plus</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
-    <t>E18</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>B12</t>
-  </si>
-  <si>
-    <t>E6_plus</t>
-  </si>
-  <si>
-    <t>E19</t>
-  </si>
-  <si>
-    <t>E20</t>
-  </si>
-  <si>
-    <t>E21</t>
-  </si>
-  <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>B14</t>
-  </si>
-  <si>
     <t>SWVersion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2187,12 +2079,23 @@
   </si>
   <si>
     <t>RootCause45</t>
+  </si>
+  <si>
+    <t>DueDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResolveDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2251,7 +2154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2267,6 +2170,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2570,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2587,11 +2493,14 @@
     <col min="8" max="8" width="15.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.06640625" style="1"/>
+    <col min="11" max="11" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -2614,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -2625,11 +2534,17 @@
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -2652,22 +2567,28 @@
         <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>365</v>
+      </c>
+      <c r="L2" s="6">
+        <v>43265</v>
+      </c>
+      <c r="M2" s="6">
+        <v>43265</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>150</v>
       </c>
@@ -2690,22 +2611,28 @@
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>390</v>
+        <v>354</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>366</v>
+      </c>
+      <c r="L3" s="6">
+        <v>43265.041666666664</v>
+      </c>
+      <c r="M3" s="6">
+        <v>43265</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>151</v>
       </c>
@@ -2728,22 +2655,28 @@
         <v>25</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>371</v>
+        <v>335</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="L4" s="6">
+        <v>43252.083333333336</v>
+      </c>
+      <c r="M4" s="6">
+        <v>43252</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>152</v>
       </c>
@@ -2766,22 +2699,28 @@
         <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>372</v>
+        <v>336</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L5" s="6">
+        <v>43253.125</v>
+      </c>
+      <c r="M5" s="6">
+        <v>43253</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>153</v>
       </c>
@@ -2804,22 +2743,28 @@
         <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>373</v>
+        <v>337</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="L6" s="6">
+        <v>43254.166666666664</v>
+      </c>
+      <c r="M6" s="6">
+        <v>43254</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>154</v>
       </c>
@@ -2842,22 +2787,28 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>374</v>
+        <v>338</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="L7" s="6">
+        <v>43255.208333333336</v>
+      </c>
+      <c r="M7" s="6">
+        <v>43255</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>155</v>
       </c>
@@ -2880,22 +2831,28 @@
         <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>375</v>
+        <v>339</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="L8" s="6">
+        <v>43256.25</v>
+      </c>
+      <c r="M8" s="6">
+        <v>43256</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>156</v>
       </c>
@@ -2918,22 +2875,28 @@
         <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="L9" s="6">
+        <v>43257.291666666664</v>
+      </c>
+      <c r="M9" s="6">
+        <v>43257</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>157</v>
       </c>
@@ -2953,25 +2916,31 @@
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>377</v>
+        <v>341</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L10" s="6">
+        <v>43258.333333333336</v>
+      </c>
+      <c r="M10" s="6">
+        <v>43258</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>158</v>
       </c>
@@ -2991,25 +2960,31 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>203</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>378</v>
+        <v>342</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="L11" s="6">
+        <v>43259.375</v>
+      </c>
+      <c r="M11" s="6">
+        <v>43259</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>159</v>
       </c>
@@ -3029,25 +3004,31 @@
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>204</v>
+        <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>379</v>
+        <v>343</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="L12" s="6">
+        <v>43260.416666666664</v>
+      </c>
+      <c r="M12" s="6">
+        <v>43260</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>160</v>
       </c>
@@ -3067,25 +3048,31 @@
         <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>380</v>
+        <v>344</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="L13" s="6">
+        <v>43261.458333333336</v>
+      </c>
+      <c r="M13" s="6">
+        <v>43261</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>161</v>
       </c>
@@ -3105,25 +3092,31 @@
         <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>206</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>381</v>
+        <v>345</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="L14" s="6">
+        <v>43262.5</v>
+      </c>
+      <c r="M14" s="6">
+        <v>43262</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>179</v>
       </c>
@@ -3143,25 +3136,31 @@
         <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>207</v>
+        <v>28</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>382</v>
+        <v>346</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="L15" s="6">
+        <v>43263.541666666664</v>
+      </c>
+      <c r="M15" s="6">
+        <v>43263</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>180</v>
       </c>
@@ -3181,25 +3180,31 @@
         <v>18</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>208</v>
+        <v>29</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>383</v>
+        <v>347</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="L16" s="6">
+        <v>43264.583333333336</v>
+      </c>
+      <c r="M16" s="6">
+        <v>43264</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>181</v>
       </c>
@@ -3222,22 +3227,28 @@
         <v>30</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>299</v>
+        <v>263</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>384</v>
+        <v>348</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="L17" s="6">
+        <v>43265.625</v>
+      </c>
+      <c r="M17" s="6">
+        <v>43265</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>182</v>
       </c>
@@ -3257,25 +3268,31 @@
         <v>5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>385</v>
+        <v>349</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>381</v>
+      </c>
+      <c r="L18" s="6">
+        <v>43266.666666666664</v>
+      </c>
+      <c r="M18" s="6">
+        <v>43266</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>183</v>
       </c>
@@ -3295,25 +3312,31 @@
         <v>20</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>209</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>386</v>
+        <v>350</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>382</v>
+      </c>
+      <c r="L19" s="6">
+        <v>43267.708333333336</v>
+      </c>
+      <c r="M19" s="6">
+        <v>43267</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>184</v>
       </c>
@@ -3333,25 +3356,31 @@
         <v>6</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>210</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>387</v>
+        <v>351</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>383</v>
+      </c>
+      <c r="L20" s="6">
+        <v>43268.75</v>
+      </c>
+      <c r="M20" s="6">
+        <v>43268</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>185</v>
       </c>
@@ -3371,25 +3400,31 @@
         <v>7</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>211</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>388</v>
+        <v>352</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>384</v>
+      </c>
+      <c r="L21" s="6">
+        <v>43269.791666666664</v>
+      </c>
+      <c r="M21" s="6">
+        <v>43269</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>186</v>
       </c>
@@ -3409,25 +3444,31 @@
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>212</v>
+        <v>27</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>389</v>
+        <v>353</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>385</v>
+      </c>
+      <c r="L22" s="6">
+        <v>43270.833333333336</v>
+      </c>
+      <c r="M22" s="6">
+        <v>43270</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>187</v>
       </c>
@@ -3447,25 +3488,31 @@
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>213</v>
+        <v>28</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>391</v>
+        <v>355</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>386</v>
+      </c>
+      <c r="L23" s="6">
+        <v>43271.875</v>
+      </c>
+      <c r="M23" s="6">
+        <v>43271</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>188</v>
       </c>
@@ -3485,25 +3532,31 @@
         <v>10</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>214</v>
+        <v>29</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>392</v>
+        <v>356</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>387</v>
+      </c>
+      <c r="L24" s="6">
+        <v>43272.916666666664</v>
+      </c>
+      <c r="M24" s="6">
+        <v>43272</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>189</v>
       </c>
@@ -3523,22 +3576,28 @@
         <v>30</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>393</v>
+        <v>357</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>388</v>
+      </c>
+      <c r="L25" s="6">
+        <v>43273.958333333336</v>
+      </c>
+      <c r="M25" s="6">
+        <v>43273</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>190</v>
       </c>
@@ -3555,25 +3614,31 @@
         <v>12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>394</v>
+        <v>358</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>389</v>
+      </c>
+      <c r="L26" s="6">
+        <v>43275</v>
+      </c>
+      <c r="M26" s="6">
+        <v>43274</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>191</v>
       </c>
@@ -3590,25 +3655,31 @@
         <v>13</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>215</v>
+        <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>395</v>
+        <v>359</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>390</v>
+      </c>
+      <c r="L27" s="6">
+        <v>43276.041666666664</v>
+      </c>
+      <c r="M27" s="6">
+        <v>43275</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>192</v>
       </c>
@@ -3625,117 +3696,147 @@
         <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>396</v>
+        <v>360</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>391</v>
+      </c>
+      <c r="L28" s="6">
+        <v>43277.083333333336</v>
+      </c>
+      <c r="M28" s="6">
+        <v>43276</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="F29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>217</v>
+        <v>26</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>392</v>
+      </c>
+      <c r="L29" s="6">
+        <v>43278.125</v>
+      </c>
+      <c r="M29" s="6">
+        <v>43277</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="F30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>218</v>
+        <v>27</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>398</v>
+        <v>362</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>393</v>
+      </c>
+      <c r="L30" s="6">
+        <v>43279.166666666664</v>
+      </c>
+      <c r="M30" s="6">
+        <v>43278</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>399</v>
+        <v>363</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>394</v>
+      </c>
+      <c r="L31" s="6">
+        <v>43280.208333333336</v>
+      </c>
+      <c r="M31" s="6">
+        <v>43279</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="F32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>220</v>
+        <v>29</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>400</v>
+        <v>364</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12">
+        <v>395</v>
+      </c>
+      <c r="L32" s="6">
+        <v>43281.25</v>
+      </c>
+      <c r="M32" s="6">
+        <v>43280</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="6:14">
       <c r="F33" s="1" t="s">
         <v>19</v>
       </c>
@@ -3743,144 +3844,150 @@
         <v>30</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12">
+        <v>396</v>
+      </c>
+      <c r="L33" s="6">
+        <v>43282.291666666664</v>
+      </c>
+      <c r="M33" s="6">
+        <v>43281</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14">
       <c r="F34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="35" spans="6:12">
+        <v>397</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14">
       <c r="F35" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>221</v>
+        <v>24</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="36" spans="6:12">
+        <v>398</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14">
       <c r="F36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>222</v>
+        <v>25</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="37" spans="6:12">
+        <v>282</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14">
       <c r="F37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>223</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="38" spans="6:12">
+        <v>283</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="6:14">
       <c r="F38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="39" spans="6:12">
+        <v>284</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="6:14">
       <c r="F39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>225</v>
+        <v>28</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="40" spans="6:12">
+        <v>285</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="40" spans="6:14">
       <c r="F40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>226</v>
+        <v>29</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12">
+        <v>286</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="6:14">
       <c r="F41" s="1" t="s">
         <v>11</v>
       </c>
@@ -3888,114 +3995,114 @@
         <v>30</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="42" spans="6:12">
+        <v>287</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="6:14">
       <c r="F42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="43" spans="6:12">
+        <v>288</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="43" spans="6:14">
       <c r="F43" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>227</v>
+        <v>24</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="44" spans="6:12">
+        <v>289</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="44" spans="6:14">
       <c r="F44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>228</v>
+        <v>25</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="45" spans="6:12">
+        <v>290</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="45" spans="6:14">
       <c r="F45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>229</v>
+        <v>26</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="46" spans="6:12">
+        <v>291</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="46" spans="6:14">
       <c r="F46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>230</v>
+        <v>27</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="47" spans="6:12">
+        <v>292</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="47" spans="6:14">
       <c r="F47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>231</v>
+        <v>28</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="48" spans="6:12">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="48" spans="6:14">
       <c r="F48" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>232</v>
+        <v>29</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="6:9">
@@ -4006,7 +4113,7 @@
         <v>30</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="6:9">
@@ -4014,10 +4121,10 @@
         <v>5</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>206</v>
+        <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="6:9">
@@ -4025,10 +4132,10 @@
         <v>20</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>233</v>
+        <v>24</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="6:9">
@@ -4036,10 +4143,10 @@
         <v>6</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>234</v>
+        <v>25</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>334</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="6:9">
@@ -4047,10 +4154,10 @@
         <v>7</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>235</v>
+        <v>26</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="6:9">
@@ -4058,10 +4165,10 @@
         <v>8</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>236</v>
+        <v>27</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="6:9">
@@ -4069,10 +4176,10 @@
         <v>9</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="6:9">
@@ -4080,10 +4187,10 @@
         <v>10</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>238</v>
+        <v>29</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="6:9">
@@ -4094,7 +4201,7 @@
         <v>30</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="6:9">
@@ -4102,7 +4209,7 @@
         <v>12</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
     </row>
     <row r="59" spans="6:9">
@@ -4110,7 +4217,7 @@
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="6:9">
@@ -4118,7 +4225,7 @@
         <v>14</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>342</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="6:9">
@@ -4126,7 +4233,7 @@
         <v>15</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
     </row>
     <row r="62" spans="6:9">
@@ -4134,7 +4241,7 @@
         <v>16</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="6:9">
@@ -4142,7 +4249,7 @@
         <v>17</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="6:9">
@@ -4150,7 +4257,7 @@
         <v>18</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="6:9">
@@ -4158,7 +4265,7 @@
         <v>19</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="6:9">
@@ -4166,7 +4273,7 @@
         <v>5</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>348</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="6:9">
@@ -4174,7 +4281,7 @@
         <v>20</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68" spans="6:9">
@@ -4182,7 +4289,7 @@
         <v>6</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>350</v>
+        <v>314</v>
       </c>
     </row>
     <row r="69" spans="6:9">
@@ -4190,7 +4297,7 @@
         <v>7</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
     </row>
     <row r="70" spans="6:9">
@@ -4198,7 +4305,7 @@
         <v>8</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>352</v>
+        <v>316</v>
       </c>
     </row>
     <row r="71" spans="6:9">
@@ -4206,7 +4313,7 @@
         <v>9</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>353</v>
+        <v>317</v>
       </c>
     </row>
     <row r="72" spans="6:9">
@@ -4214,7 +4321,7 @@
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>354</v>
+        <v>318</v>
       </c>
     </row>
     <row r="73" spans="6:9">
@@ -4222,7 +4329,7 @@
         <v>11</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
     </row>
     <row r="74" spans="6:9">
@@ -4230,7 +4337,7 @@
         <v>12</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="6:9">
@@ -4238,7 +4345,7 @@
         <v>13</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="6:9">
@@ -4246,7 +4353,7 @@
         <v>14</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="6:9">
@@ -4254,7 +4361,7 @@
         <v>15</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="78" spans="6:9">
@@ -4262,7 +4369,7 @@
         <v>16</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>360</v>
+        <v>324</v>
       </c>
     </row>
     <row r="79" spans="6:9">
@@ -4270,7 +4377,7 @@
         <v>17</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
     </row>
     <row r="80" spans="6:9">
@@ -4278,7 +4385,7 @@
         <v>18</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>362</v>
+        <v>326</v>
       </c>
     </row>
     <row r="81" spans="6:9">
@@ -4286,7 +4393,7 @@
         <v>19</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>363</v>
+        <v>327</v>
       </c>
     </row>
     <row r="82" spans="6:9">
@@ -4294,7 +4401,7 @@
         <v>5</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83" spans="6:9">
@@ -4302,7 +4409,7 @@
         <v>20</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>365</v>
+        <v>329</v>
       </c>
     </row>
     <row r="84" spans="6:9">
@@ -4310,7 +4417,7 @@
         <v>6</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>366</v>
+        <v>330</v>
       </c>
     </row>
     <row r="85" spans="6:9">
@@ -4318,7 +4425,7 @@
         <v>7</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>367</v>
+        <v>331</v>
       </c>
     </row>
     <row r="86" spans="6:9">
@@ -4326,7 +4433,7 @@
         <v>8</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
     </row>
     <row r="87" spans="6:9">
@@ -4334,7 +4441,7 @@
         <v>9</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>369</v>
+        <v>333</v>
       </c>
     </row>
     <row r="88" spans="6:9">
@@ -4379,7 +4486,7 @@
   <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>